<commit_message>
added files to report and compile target, updated formatTables with font opts
</commit_message>
<xml_diff>
--- a/tables/tables.xlsx
+++ b/tables/tables.xlsx
@@ -641,18 +641,18 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="GDS Transport Website"/>
+      <name val="Arial"/>
       <b/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
-      <name val="GDS Transport Website"/>
+      <name val="Arial"/>
     </font>
     <font>
       <sz val="16"/>
       <color rgb="FF000000"/>
-      <name val="GDS Transport Website"/>
+      <name val="Arial"/>
       <b/>
     </font>
     <font>
@@ -663,13 +663,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF808080"/>
-      <name val="GDS Transport Website"/>
+      <name val="Arial"/>
       <b/>
     </font>
     <font>
       <sz val="11"/>
       <color rgb="FF808080"/>
-      <name val="GDS Transport Website"/>
+      <name val="Arial"/>
     </font>
   </fonts>
   <fills count="3">

</xml_diff>